<commit_message>
auth page corrected. Slight UI modications to Dashboard.
</commit_message>
<xml_diff>
--- a/data/New_Query_2025_07_21_11_13am.xlsx
+++ b/data/New_Query_2025_07_21_11_13am.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Anshul_Agarwal/Library/CloudStorage/Box-Box/DCM/99 Working folders/14 Anshul/Margin Maximizer/h2_margin_maximizer/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68EA57C3-29D9-764D-AFCB-721DB2D2970A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37A216F-100E-D24A-B2E0-3FE97F68E0B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="34200" windowHeight="19660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -324,7 +324,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -357,7 +357,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -699,7 +699,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CT11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CH1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="CL1" zoomScale="125" workbookViewId="0">
       <selection activeCell="CT2" sqref="CT2"/>
     </sheetView>
   </sheetViews>
@@ -3966,8 +3966,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:CT11" numberStoredAsText="1"/>
+    <ignoredError sqref="A2:CT11 A1:CP1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>